<commit_message>
updated with Q1 2025 results for property
</commit_message>
<xml_diff>
--- a/data/Property_Metrics.xlsx
+++ b/data/Property_Metrics.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D201"/>
+  <dimension ref="A1:D237"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -4379,6 +4379,726 @@
         </is>
       </c>
     </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>Combined Ratio</t>
+        </is>
+      </c>
+      <c r="B202">
+        <v>91</v>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D202" t="inlineStr">
+        <is>
+          <t>Q1 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>Combined Ratio</t>
+        </is>
+      </c>
+      <c r="B203">
+        <v>94.09999999999999</v>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D203" t="inlineStr">
+        <is>
+          <t>Q1 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>Claims Ratio</t>
+        </is>
+      </c>
+      <c r="B204">
+        <v>59.9</v>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D204" t="inlineStr">
+        <is>
+          <t>Q1 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>Claims Ratio</t>
+        </is>
+      </c>
+      <c r="B205">
+        <v>55.2</v>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>Q1 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>Core Claim Ratio</t>
+        </is>
+      </c>
+      <c r="B206">
+        <v>51.3</v>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D206" t="inlineStr">
+        <is>
+          <t>Q1 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>Core Claim Ratio</t>
+        </is>
+      </c>
+      <c r="B207">
+        <v>52</v>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D207" t="inlineStr">
+        <is>
+          <t>Q1 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>CAT Loss Ratio</t>
+        </is>
+      </c>
+      <c r="B208">
+        <v>11.8</v>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>Q1 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>CAT Loss Ratio</t>
+        </is>
+      </c>
+      <c r="B209">
+        <v>5.9</v>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>Q1 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>Expense Ratio</t>
+        </is>
+      </c>
+      <c r="B210">
+        <v>35.8</v>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>Q1 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>Expense Ratio</t>
+        </is>
+      </c>
+      <c r="B211">
+        <v>34.2</v>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>Q1 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>PYD Ratio</t>
+        </is>
+      </c>
+      <c r="B212">
+        <v>-3.9</v>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>Q1 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>PYD Ratio</t>
+        </is>
+      </c>
+      <c r="B213">
+        <v>-2</v>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>Q1 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>Gross Written Premium</t>
+        </is>
+      </c>
+      <c r="B214">
+        <v>236.5</v>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>Q1 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>Gross Written Premium</t>
+        </is>
+      </c>
+      <c r="B215">
+        <v>255</v>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>Q1 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>Underwriting Income</t>
+        </is>
+      </c>
+      <c r="B216">
+        <v>16.8</v>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>Q1 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>Underwriting Income</t>
+        </is>
+      </c>
+      <c r="B217">
+        <v>23.5</v>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>Q1 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>ROE</t>
+        </is>
+      </c>
+      <c r="B218">
+        <v>9.5</v>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>Q1 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>ROE</t>
+        </is>
+      </c>
+      <c r="B219">
+        <v>10.3</v>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>Definity</t>
+        </is>
+      </c>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>Q1 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>Combined Ratio</t>
+        </is>
+      </c>
+      <c r="B220">
+        <v>88.90000000000001</v>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>Q1 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>Combined Ratio</t>
+        </is>
+      </c>
+      <c r="B221">
+        <v>82.5</v>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>Q1 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>Claims Ratio</t>
+        </is>
+      </c>
+      <c r="B222">
+        <v>46.4</v>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>Q1 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>Claims Ratio</t>
+        </is>
+      </c>
+      <c r="B223">
+        <v>55.6</v>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>Q1 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>Core Claim Ratio</t>
+        </is>
+      </c>
+      <c r="B224">
+        <v>53.7</v>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>Q1 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>Core Claim Ratio</t>
+        </is>
+      </c>
+      <c r="B225">
+        <v>51</v>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D225" t="inlineStr">
+        <is>
+          <t>Q1 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>CAT Loss Ratio</t>
+        </is>
+      </c>
+      <c r="B226">
+        <v>0</v>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D226" t="inlineStr">
+        <is>
+          <t>Q1 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>CAT Loss Ratio</t>
+        </is>
+      </c>
+      <c r="B227">
+        <v>7.5</v>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D227" t="inlineStr">
+        <is>
+          <t>Q1 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>Expense Ratio</t>
+        </is>
+      </c>
+      <c r="B228">
+        <v>33.3</v>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D228" t="inlineStr">
+        <is>
+          <t>Q1 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>Expense Ratio</t>
+        </is>
+      </c>
+      <c r="B229">
+        <v>36.1</v>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D229" t="inlineStr">
+        <is>
+          <t>Q1 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>PYD Ratio</t>
+        </is>
+      </c>
+      <c r="B230">
+        <v>-4.6</v>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D230" t="inlineStr">
+        <is>
+          <t>Q1 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>PYD Ratio</t>
+        </is>
+      </c>
+      <c r="B231">
+        <v>-5.6</v>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D231" t="inlineStr">
+        <is>
+          <t>Q1 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>Gross Written Premium</t>
+        </is>
+      </c>
+      <c r="B232">
+        <v>903</v>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D232" t="inlineStr">
+        <is>
+          <t>Q1 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>Gross Written Premium</t>
+        </is>
+      </c>
+      <c r="B233">
+        <v>828</v>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D233" t="inlineStr">
+        <is>
+          <t>Q1 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>Underwriting Income</t>
+        </is>
+      </c>
+      <c r="B234">
+        <v>166</v>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D234" t="inlineStr">
+        <is>
+          <t>Q1 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>Underwriting Income</t>
+        </is>
+      </c>
+      <c r="B235">
+        <v>113</v>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D235" t="inlineStr">
+        <is>
+          <t>Q1 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>ROE</t>
+        </is>
+      </c>
+      <c r="B236">
+        <v>13.7</v>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D236" t="inlineStr">
+        <is>
+          <t>Q1 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>ROE</t>
+        </is>
+      </c>
+      <c r="B237">
+        <v>10.6</v>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>Intact</t>
+        </is>
+      </c>
+      <c r="D237" t="inlineStr">
+        <is>
+          <t>Q1 2024</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>